<commit_message>
calculateConfidence refactored - names, annotations & sequences
</commit_message>
<xml_diff>
--- a/Data/Exports/Invoice 0000007.pdf_1-1.xlsx
+++ b/Data/Exports/Invoice 0000007.pdf_1-1.xlsx
@@ -191,7 +191,19 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="32">
+  <x:cellStyleXfs count="36">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>

<commit_message>
Confidence of table items added
</commit_message>
<xml_diff>
--- a/Data/Exports/Invoice 0000007.pdf_1-1.xlsx
+++ b/Data/Exports/Invoice 0000007.pdf_1-1.xlsx
@@ -191,7 +191,43 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="36">
+  <x:cellStyleXfs count="48">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>